<commit_message>
preprocessing case folding , remove mention and link and lin breaks
</commit_message>
<xml_diff>
--- a/dataset/test.xlsx
+++ b/dataset/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arya Enrico\Downloads\paper review\skripsi\program\preprocessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0E7F32-4156-4260-9C1B-58330A645EE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72820A5-2F7E-49CB-B786-7E7BEE92C316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Tanggal</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t xml:space="preserve">anjing lu china tolol bunuh aja </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tolol banget ini orang @aryaenrico https://t.co/x7kIgg2VXH </t>
+  </si>
+  <si>
+    <t>nhs</t>
   </si>
 </sst>
 </file>
@@ -359,10 +365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -404,6 +410,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>45009</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
create database and insert expample of slangword
</commit_message>
<xml_diff>
--- a/dataset/test.xlsx
+++ b/dataset/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arya Enrico\Downloads\paper review\skripsi\program\preprocessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF327F7A-B663-4E5B-88B9-849F7CE73E4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DDE5D4-51F2-4463-94A2-F24BBE33A30C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="9">
   <si>
     <t>Tanggal</t>
   </si>
@@ -375,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103:C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -443,6 +443,1117 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
+        <v>45009</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
+        <v>45010</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1">
+        <v>45009</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1">
+        <v>45010</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1">
+        <v>45009</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1">
+        <v>45010</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1">
+        <v>45009</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1">
+        <v>45010</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1">
+        <v>45009</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1">
+        <v>45010</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="1">
+        <v>45009</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="1">
+        <v>45010</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="1">
+        <v>45009</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="1">
+        <v>45010</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="1">
+        <v>45009</v>
+      </c>
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="1">
+        <v>45010</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="1">
+        <v>45009</v>
+      </c>
+      <c r="B40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="1">
+        <v>45010</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="1">
+        <v>45009</v>
+      </c>
+      <c r="B44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="1">
+        <v>45010</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B47" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="1">
+        <v>45009</v>
+      </c>
+      <c r="B48" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="1">
+        <v>45010</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="1">
+        <v>45009</v>
+      </c>
+      <c r="B52" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="1">
+        <v>45010</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B55" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="1">
+        <v>45009</v>
+      </c>
+      <c r="B56" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="1">
+        <v>45010</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B59" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="1">
+        <v>45009</v>
+      </c>
+      <c r="B60" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="1">
+        <v>45010</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B63" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="1">
+        <v>45009</v>
+      </c>
+      <c r="B64" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="1">
+        <v>45010</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B67" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="1">
+        <v>45009</v>
+      </c>
+      <c r="B68" t="s">
+        <v>6</v>
+      </c>
+      <c r="C68" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="1">
+        <v>45010</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C69" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B71" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="1">
+        <v>45009</v>
+      </c>
+      <c r="B72" t="s">
+        <v>6</v>
+      </c>
+      <c r="C72" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="1">
+        <v>45010</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B75" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="1">
+        <v>45009</v>
+      </c>
+      <c r="B76" t="s">
+        <v>6</v>
+      </c>
+      <c r="C76" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="1">
+        <v>45010</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C77" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B79" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="1">
+        <v>45009</v>
+      </c>
+      <c r="B80" t="s">
+        <v>6</v>
+      </c>
+      <c r="C80" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="1">
+        <v>45010</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C81" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="1">
+        <v>45010</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B84" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="1">
+        <v>45009</v>
+      </c>
+      <c r="B85" t="s">
+        <v>6</v>
+      </c>
+      <c r="C85" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="1">
+        <v>45010</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C86" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B88" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="1">
+        <v>45009</v>
+      </c>
+      <c r="B89" t="s">
+        <v>6</v>
+      </c>
+      <c r="C89" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="1">
+        <v>45010</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C90" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B92" t="s">
+        <v>5</v>
+      </c>
+      <c r="C92" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="1">
+        <v>45009</v>
+      </c>
+      <c r="B93" t="s">
+        <v>6</v>
+      </c>
+      <c r="C93" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="1">
+        <v>45010</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C94" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B96" t="s">
+        <v>5</v>
+      </c>
+      <c r="C96" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="1">
+        <v>45009</v>
+      </c>
+      <c r="B97" t="s">
+        <v>6</v>
+      </c>
+      <c r="C97" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="1">
+        <v>45010</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C98" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B100" t="s">
+        <v>5</v>
+      </c>
+      <c r="C100" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="1">
+        <v>45009</v>
+      </c>
+      <c r="B101" t="s">
+        <v>6</v>
+      </c>
+      <c r="C101" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="1">
+        <v>45010</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C102" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B104" t="s">
+        <v>5</v>
+      </c>
+      <c r="C104" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="1">
+        <v>45009</v>
+      </c>
+      <c r="B105" t="s">
+        <v>6</v>
+      </c>
+      <c r="C105" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="1">
+        <v>45010</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C106" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>